<commit_message>
added additional costal locations
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/gigok_trial.xlsx
+++ b/analysis/data/raw_data/gigok_trial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gayoungp/koreapaleolithicmobilityoccupation/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{046D78A6-8BA4-0D4B-8CE6-8EB056325BE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AB9635-4307-9B40-AA9D-C2EA5838CBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="1860" windowWidth="14020" windowHeight="14140" xr2:uid="{B88E52FE-D889-174E-8EE1-FD39967D1B8E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>site_name</t>
   </si>
@@ -66,6 +66,33 @@
   </si>
   <si>
     <t>far_C</t>
+  </si>
+  <si>
+    <t>cost_A</t>
+  </si>
+  <si>
+    <t>cost_B</t>
+  </si>
+  <si>
+    <t>cost_C</t>
+  </si>
+  <si>
+    <t>cost_D</t>
+  </si>
+  <si>
+    <t>cost_E</t>
+  </si>
+  <si>
+    <t>cost_F</t>
+  </si>
+  <si>
+    <t>cost_G</t>
+  </si>
+  <si>
+    <t>cost_H</t>
+  </si>
+  <si>
+    <t>cost_I</t>
   </si>
 </sst>
 </file>
@@ -417,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7943044-CC59-EB43-8EDC-FE95C91AA6BA}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -524,6 +551,105 @@
         <v>128.64224999999999</v>
       </c>
     </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>37.689441000000002</v>
+      </c>
+      <c r="C10">
+        <v>129.03623099999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>37.640802000000001</v>
+      </c>
+      <c r="C11">
+        <v>129.044299</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12">
+        <v>37.599268000000002</v>
+      </c>
+      <c r="C12">
+        <v>129.082065</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13">
+        <v>37.556690000000003</v>
+      </c>
+      <c r="C13">
+        <v>129.12120400000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>37.511091999999998</v>
+      </c>
+      <c r="C14">
+        <v>129.12944400000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>37.402901</v>
+      </c>
+      <c r="C15">
+        <v>129.21115499999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>37.342744000000003</v>
+      </c>
+      <c r="C16">
+        <v>129.26574299999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>37.160060000000001</v>
+      </c>
+      <c r="C17">
+        <v>129.355694</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>36.980088000000002</v>
+      </c>
+      <c r="C18">
+        <v>129.40719200000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added boxplot for Gigok trial and annotations for the climate line plot
</commit_message>
<xml_diff>
--- a/analysis/data/raw_data/gigok_trial.xlsx
+++ b/analysis/data/raw_data/gigok_trial.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gayoungp/koreapaleolithicmobilityoccupation/analysis/data/raw_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AB9635-4307-9B40-AA9D-C2EA5838CBC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31B04F8-301A-7A40-BAC1-187213AF0BE7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4320" yWindow="1860" windowWidth="14020" windowHeight="14140" xr2:uid="{B88E52FE-D889-174E-8EE1-FD39967D1B8E}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -652,5 +652,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>